<commit_message>
opdatering af risk management
</commit_message>
<xml_diff>
--- a/Dokumenter/Risk management.xlsx
+++ b/Dokumenter/Risk management.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Identified Risks</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Hardware</t>
   </si>
 </sst>
 </file>
@@ -159,12 +165,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Besøgt link" xfId="2" builtinId="9" hidden="1"/>
@@ -247,10 +255,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ark1'!$C$2:$C$7</c:f>
+              <c:f>'Ark1'!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -268,16 +276,22 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ark1'!$D$2:$D$7</c:f>
+              <c:f>'Ark1'!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -295,6 +309,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -309,11 +329,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="42576128"/>
-        <c:axId val="42574592"/>
+        <c:axId val="31433856"/>
+        <c:axId val="31435392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42576128"/>
+        <c:axId val="31433856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -323,12 +343,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42574592"/>
+        <c:crossAx val="31435392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42574592"/>
+        <c:axId val="31435392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -339,7 +359,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42576128"/>
+        <c:crossAx val="31433856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -713,17 +733,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="55.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -828,8 +848,29 @@
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>